<commit_message>
Maps Code made generic
</commit_message>
<xml_diff>
--- a/my-Solution/src/main/java/com/outputFiles/repository/LocationDetails.xlsx
+++ b/my-Solution/src/main/java/com/outputFiles/repository/LocationDetails.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{97CB2640-45E7-465B-A4E4-C2A7C6284255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" r:id="rId3" sheetId="1"/>
+    <sheet name="Locations" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="56">
   <si>
     <t>National Hardware redevelopment</t>
   </si>
@@ -185,11 +189,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -201,7 +204,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -219,20 +222,333 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CD46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -262,9 +578,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -321,9 +637,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -380,9 +696,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -466,9 +782,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -552,9 +868,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -568,9 +884,6 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -638,9 +951,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -654,9 +967,6 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
@@ -751,9 +1061,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -767,9 +1077,6 @@
       <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
@@ -864,9 +1171,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -880,9 +1187,6 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
@@ -977,9 +1281,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -993,9 +1297,6 @@
       <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
@@ -1090,9 +1391,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1106,9 +1407,6 @@
       <c r="E12" t="s">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
@@ -1230,9 +1528,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1246,9 +1544,6 @@
       <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>4</v>
-      </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
@@ -1370,9 +1665,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1386,9 +1681,6 @@
       <c r="E14" t="s">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>4</v>
-      </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -1510,9 +1802,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -1526,9 +1818,6 @@
       <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="F15" t="s">
-        <v>4</v>
-      </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
@@ -1650,9 +1939,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -1666,9 +1955,6 @@
       <c r="E16" t="s">
         <v>3</v>
       </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
@@ -1790,9 +2076,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -1806,9 +2092,6 @@
       <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="F17" t="s">
-        <v>4</v>
-      </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
@@ -1957,9 +2240,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -1973,9 +2256,6 @@
       <c r="E18" t="s">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>4</v>
-      </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
@@ -2124,9 +2404,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -2140,9 +2420,6 @@
       <c r="E19" t="s">
         <v>3</v>
       </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
@@ -2291,9 +2568,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -2307,9 +2584,6 @@
       <c r="E20" t="s">
         <v>3</v>
       </c>
-      <c r="F20" t="s">
-        <v>4</v>
-      </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
@@ -2458,9 +2732,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -2474,9 +2748,6 @@
       <c r="E21" t="s">
         <v>3</v>
       </c>
-      <c r="F21" t="s">
-        <v>4</v>
-      </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
@@ -2625,9 +2896,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2641,9 +2912,6 @@
       <c r="E22" t="s">
         <v>3</v>
       </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
@@ -2792,9 +3060,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -2808,9 +3076,6 @@
       <c r="E23" t="s">
         <v>3</v>
       </c>
-      <c r="F23" t="s">
-        <v>4</v>
-      </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
@@ -2986,9 +3251,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -3002,9 +3267,6 @@
       <c r="E24" t="s">
         <v>3</v>
       </c>
-      <c r="F24" t="s">
-        <v>4</v>
-      </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
@@ -3180,9 +3442,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -3196,9 +3458,6 @@
       <c r="E25" t="s">
         <v>3</v>
       </c>
-      <c r="F25" t="s">
-        <v>4</v>
-      </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -3374,9 +3633,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -3390,9 +3649,6 @@
       <c r="E26" t="s">
         <v>3</v>
       </c>
-      <c r="F26" t="s">
-        <v>4</v>
-      </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
@@ -3568,9 +3824,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -3584,9 +3840,6 @@
       <c r="E27" t="s">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
@@ -3762,9 +4015,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -3778,9 +4031,6 @@
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="F28" t="s">
-        <v>4</v>
-      </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
@@ -3956,9 +4206,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -3972,9 +4222,6 @@
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="F29" t="s">
-        <v>4</v>
-      </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
@@ -4150,9 +4397,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -4166,9 +4413,6 @@
       <c r="E30" t="s">
         <v>3</v>
       </c>
-      <c r="F30" t="s">
-        <v>4</v>
-      </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -4371,9 +4615,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -4387,9 +4631,6 @@
       <c r="E31" t="s">
         <v>3</v>
       </c>
-      <c r="F31" t="s">
-        <v>4</v>
-      </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
@@ -4592,9 +4833,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -4608,9 +4849,6 @@
       <c r="E32" t="s">
         <v>3</v>
       </c>
-      <c r="F32" t="s">
-        <v>4</v>
-      </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
@@ -4813,9 +5051,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -4829,9 +5067,6 @@
       <c r="E33" t="s">
         <v>3</v>
       </c>
-      <c r="F33" t="s">
-        <v>4</v>
-      </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
@@ -5034,9 +5269,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -5050,9 +5285,6 @@
       <c r="E34" t="s">
         <v>3</v>
       </c>
-      <c r="F34" t="s">
-        <v>4</v>
-      </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
@@ -5255,9 +5487,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -5271,9 +5503,6 @@
       <c r="E35" t="s">
         <v>3</v>
       </c>
-      <c r="F35" t="s">
-        <v>4</v>
-      </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -5476,9 +5705,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -5492,9 +5721,6 @@
       <c r="E36" t="s">
         <v>3</v>
       </c>
-      <c r="F36" t="s">
-        <v>4</v>
-      </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
@@ -5697,9 +5923,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -5713,9 +5939,6 @@
       <c r="E37" t="s">
         <v>3</v>
       </c>
-      <c r="F37" t="s">
-        <v>4</v>
-      </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
@@ -5918,9 +6141,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -5934,9 +6157,6 @@
       <c r="E38" t="s">
         <v>3</v>
       </c>
-      <c r="F38" t="s">
-        <v>4</v>
-      </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
@@ -6166,9 +6386,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -6182,9 +6402,6 @@
       <c r="E39" t="s">
         <v>3</v>
       </c>
-      <c r="F39" t="s">
-        <v>4</v>
-      </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
@@ -6414,9 +6631,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -6430,9 +6647,6 @@
       <c r="E40" t="s">
         <v>3</v>
       </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
@@ -6662,7 +6876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -6678,9 +6892,6 @@
       <c r="E41" t="s">
         <v>3</v>
       </c>
-      <c r="F41" t="s">
-        <v>4</v>
-      </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
@@ -6910,7 +7121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -6926,9 +7137,6 @@
       <c r="E42" t="s">
         <v>3</v>
       </c>
-      <c r="F42" t="s">
-        <v>4</v>
-      </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
@@ -7158,7 +7366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -7174,9 +7382,6 @@
       <c r="E43" t="s">
         <v>3</v>
       </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
@@ -7406,7 +7611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -7422,9 +7627,6 @@
       <c r="E44" t="s">
         <v>3</v>
       </c>
-      <c r="F44" t="s">
-        <v>4</v>
-      </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
@@ -7654,7 +7856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -7670,9 +7872,6 @@
       <c r="E45" t="s">
         <v>3</v>
       </c>
-      <c r="F45" t="s">
-        <v>4</v>
-      </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
@@ -7902,7 +8101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -7918,9 +8117,6 @@
       <c r="E46" t="s">
         <v>3</v>
       </c>
-      <c r="F46" t="s">
-        <v>4</v>
-      </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
@@ -8151,6 +8347,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>